<commit_message>
", ' exception code
</commit_message>
<xml_diff>
--- a/Map/excel.xlsx
+++ b/Map/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yyi07\OneDrive\문서\git\sc-musicOS\Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575F45FC-1CEF-4B9B-BDCD-098E31CEC0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C529DF-F63D-4169-B9D9-1E4A7AFC6C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2158,7 +2158,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G26:G27"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>